<commit_message>
Added simpler parsing functionality
</commit_message>
<xml_diff>
--- a/example_output.xlsx
+++ b/example_output.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:A26"/>
+  <dimension ref="A1:D25"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -436,20 +436,65 @@
     <row r="1">
       <c r="A1" s="1" t="inlineStr">
         <is>
-          <t>```csv</t>
+          <t>Rep Firm Name</t>
+        </is>
+      </c>
+      <c r="B1" s="1" t="inlineStr">
+        <is>
+          <t>Brand Carried</t>
+        </is>
+      </c>
+      <c r="C1" s="1" t="inlineStr">
+        <is>
+          <t>Product Covered</t>
+        </is>
+      </c>
+      <c r="D1" s="1" t="inlineStr">
+        <is>
+          <t>Product Space</t>
         </is>
       </c>
     </row>
     <row r="2">
       <c r="A2" t="inlineStr">
         <is>
-          <t>Product Space</t>
+          <t>Example Rep Firm</t>
+        </is>
+      </c>
+      <c r="B2" t="inlineStr">
+        <is>
+          <t>ABB</t>
+        </is>
+      </c>
+      <c r="C2" t="inlineStr">
+        <is>
+          <t>Variable Frequency Drives</t>
+        </is>
+      </c>
+      <c r="D2" t="inlineStr">
+        <is>
+          <t>Flow Control</t>
         </is>
       </c>
     </row>
     <row r="3">
       <c r="A3" t="inlineStr">
         <is>
+          <t>Example Rep Firm</t>
+        </is>
+      </c>
+      <c r="B3" t="inlineStr">
+        <is>
+          <t>Old Castle</t>
+        </is>
+      </c>
+      <c r="C3" t="inlineStr">
+        <is>
+          <t>One Lift Package Pump Station</t>
+        </is>
+      </c>
+      <c r="D3" t="inlineStr">
+        <is>
           <t>Flow Control</t>
         </is>
       </c>
@@ -457,6 +502,21 @@
     <row r="4">
       <c r="A4" t="inlineStr">
         <is>
+          <t>Example Rep Firm</t>
+        </is>
+      </c>
+      <c r="B4" t="inlineStr">
+        <is>
+          <t>Netzsch</t>
+        </is>
+      </c>
+      <c r="C4" t="inlineStr">
+        <is>
+          <t>Progressive Cavity Pumps</t>
+        </is>
+      </c>
+      <c r="D4" t="inlineStr">
+        <is>
           <t>Flow Control</t>
         </is>
       </c>
@@ -464,6 +524,21 @@
     <row r="5">
       <c r="A5" t="inlineStr">
         <is>
+          <t>Example Rep Firm</t>
+        </is>
+      </c>
+      <c r="B5" t="inlineStr">
+        <is>
+          <t>Netzsch</t>
+        </is>
+      </c>
+      <c r="C5" t="inlineStr">
+        <is>
+          <t>Rotary Lobe Pumps</t>
+        </is>
+      </c>
+      <c r="D5" t="inlineStr">
+        <is>
           <t>Flow Control</t>
         </is>
       </c>
@@ -471,13 +546,43 @@
     <row r="6">
       <c r="A6" t="inlineStr">
         <is>
-          <t>Flow Control</t>
+          <t>Example Rep Firm</t>
+        </is>
+      </c>
+      <c r="B6" t="inlineStr">
+        <is>
+          <t>USCP</t>
+        </is>
+      </c>
+      <c r="C6" t="inlineStr">
+        <is>
+          <t>Steel Reinforced Polymer Concrete Manholes</t>
+        </is>
+      </c>
+      <c r="D6" t="inlineStr">
+        <is>
+          <t>Water Treatment</t>
         </is>
       </c>
     </row>
     <row r="7">
       <c r="A7" t="inlineStr">
         <is>
+          <t>Example Rep Firm</t>
+        </is>
+      </c>
+      <c r="B7" t="inlineStr">
+        <is>
+          <t>USCP</t>
+        </is>
+      </c>
+      <c r="C7" t="inlineStr">
+        <is>
+          <t>Microtunnel Pipe</t>
+        </is>
+      </c>
+      <c r="D7" t="inlineStr">
+        <is>
           <t>Water Treatment</t>
         </is>
       </c>
@@ -485,6 +590,21 @@
     <row r="8">
       <c r="A8" t="inlineStr">
         <is>
+          <t>Example Rep Firm</t>
+        </is>
+      </c>
+      <c r="B8" t="inlineStr">
+        <is>
+          <t>USCP</t>
+        </is>
+      </c>
+      <c r="C8" t="inlineStr">
+        <is>
+          <t>Industrial Pipe Structures</t>
+        </is>
+      </c>
+      <c r="D8" t="inlineStr">
+        <is>
           <t>Water Treatment</t>
         </is>
       </c>
@@ -492,27 +612,87 @@
     <row r="9">
       <c r="A9" t="inlineStr">
         <is>
-          <t>Water Treatment</t>
+          <t>Example Rep Firm</t>
+        </is>
+      </c>
+      <c r="B9" t="inlineStr">
+        <is>
+          <t>Flygt</t>
+        </is>
+      </c>
+      <c r="C9" t="inlineStr">
+        <is>
+          <t>Submersible Pumps</t>
+        </is>
+      </c>
+      <c r="D9" t="inlineStr">
+        <is>
+          <t>Flow Control</t>
         </is>
       </c>
     </row>
     <row r="10">
       <c r="A10" t="inlineStr">
         <is>
-          <t>Flow Control</t>
+          <t>Example Rep Firm</t>
+        </is>
+      </c>
+      <c r="B10" t="inlineStr">
+        <is>
+          <t>Flygt</t>
+        </is>
+      </c>
+      <c r="C10" t="inlineStr">
+        <is>
+          <t>Mixers</t>
+        </is>
+      </c>
+      <c r="D10" t="inlineStr">
+        <is>
+          <t>Aeration</t>
         </is>
       </c>
     </row>
     <row r="11">
       <c r="A11" t="inlineStr">
         <is>
-          <t>Aeration</t>
+          <t>Example Rep Firm</t>
+        </is>
+      </c>
+      <c r="B11" t="inlineStr">
+        <is>
+          <t>Flygt</t>
+        </is>
+      </c>
+      <c r="C11" t="inlineStr">
+        <is>
+          <t>Controls</t>
+        </is>
+      </c>
+      <c r="D11" t="inlineStr">
+        <is>
+          <t>Flow Control</t>
         </is>
       </c>
     </row>
     <row r="12">
       <c r="A12" t="inlineStr">
         <is>
+          <t>Example Rep Firm</t>
+        </is>
+      </c>
+      <c r="B12" t="inlineStr">
+        <is>
+          <t>Flygt</t>
+        </is>
+      </c>
+      <c r="C12" t="inlineStr">
+        <is>
+          <t>Check Valves</t>
+        </is>
+      </c>
+      <c r="D12" t="inlineStr">
+        <is>
           <t>Flow Control</t>
         </is>
       </c>
@@ -520,6 +700,21 @@
     <row r="13">
       <c r="A13" t="inlineStr">
         <is>
+          <t>Example Rep Firm</t>
+        </is>
+      </c>
+      <c r="B13" t="inlineStr">
+        <is>
+          <t>Flygt</t>
+        </is>
+      </c>
+      <c r="C13" t="inlineStr">
+        <is>
+          <t>Mix-Flush Valves</t>
+        </is>
+      </c>
+      <c r="D13" t="inlineStr">
+        <is>
           <t>Flow Control</t>
         </is>
       </c>
@@ -527,6 +722,21 @@
     <row r="14">
       <c r="A14" t="inlineStr">
         <is>
+          <t>Example Rep Firm</t>
+        </is>
+      </c>
+      <c r="B14" t="inlineStr">
+        <is>
+          <t>ITT Gould Pumps</t>
+        </is>
+      </c>
+      <c r="C14" t="inlineStr">
+        <is>
+          <t>Standard Cast Iron Pumps</t>
+        </is>
+      </c>
+      <c r="D14" t="inlineStr">
+        <is>
           <t>Flow Control</t>
         </is>
       </c>
@@ -534,6 +744,21 @@
     <row r="15">
       <c r="A15" t="inlineStr">
         <is>
+          <t>Example Rep Firm</t>
+        </is>
+      </c>
+      <c r="B15" t="inlineStr">
+        <is>
+          <t>ITT Gould Pumps</t>
+        </is>
+      </c>
+      <c r="C15" t="inlineStr">
+        <is>
+          <t>Bronze Pumps</t>
+        </is>
+      </c>
+      <c r="D15" t="inlineStr">
+        <is>
           <t>Flow Control</t>
         </is>
       </c>
@@ -541,6 +766,21 @@
     <row r="16">
       <c r="A16" t="inlineStr">
         <is>
+          <t>Example Rep Firm</t>
+        </is>
+      </c>
+      <c r="B16" t="inlineStr">
+        <is>
+          <t>ITT Gould Pumps</t>
+        </is>
+      </c>
+      <c r="C16" t="inlineStr">
+        <is>
+          <t>End Suction Pumps</t>
+        </is>
+      </c>
+      <c r="D16" t="inlineStr">
+        <is>
           <t>Flow Control</t>
         </is>
       </c>
@@ -548,6 +788,21 @@
     <row r="17">
       <c r="A17" t="inlineStr">
         <is>
+          <t>Example Rep Firm</t>
+        </is>
+      </c>
+      <c r="B17" t="inlineStr">
+        <is>
+          <t>ITT Gould Pumps</t>
+        </is>
+      </c>
+      <c r="C17" t="inlineStr">
+        <is>
+          <t>Vertical Turbine Pumps</t>
+        </is>
+      </c>
+      <c r="D17" t="inlineStr">
+        <is>
           <t>Flow Control</t>
         </is>
       </c>
@@ -555,6 +810,21 @@
     <row r="18">
       <c r="A18" t="inlineStr">
         <is>
+          <t>Example Rep Firm</t>
+        </is>
+      </c>
+      <c r="B18" t="inlineStr">
+        <is>
+          <t>ITT Gould Pumps</t>
+        </is>
+      </c>
+      <c r="C18" t="inlineStr">
+        <is>
+          <t>Split Case Pumps</t>
+        </is>
+      </c>
+      <c r="D18" t="inlineStr">
+        <is>
           <t>Flow Control</t>
         </is>
       </c>
@@ -562,6 +832,21 @@
     <row r="19">
       <c r="A19" t="inlineStr">
         <is>
+          <t>Example Rep Firm</t>
+        </is>
+      </c>
+      <c r="B19" t="inlineStr">
+        <is>
+          <t>E/One</t>
+        </is>
+      </c>
+      <c r="C19" t="inlineStr">
+        <is>
+          <t>Packaged Low Pressure Sewer Systems</t>
+        </is>
+      </c>
+      <c r="D19" t="inlineStr">
+        <is>
           <t>Flow Control</t>
         </is>
       </c>
@@ -569,6 +854,21 @@
     <row r="20">
       <c r="A20" t="inlineStr">
         <is>
+          <t>Example Rep Firm</t>
+        </is>
+      </c>
+      <c r="B20" t="inlineStr">
+        <is>
+          <t>E/One</t>
+        </is>
+      </c>
+      <c r="C20" t="inlineStr">
+        <is>
+          <t>Collection Basin</t>
+        </is>
+      </c>
+      <c r="D20" t="inlineStr">
+        <is>
           <t>Flow Control</t>
         </is>
       </c>
@@ -576,6 +876,21 @@
     <row r="21">
       <c r="A21" t="inlineStr">
         <is>
+          <t>Example Rep Firm</t>
+        </is>
+      </c>
+      <c r="B21" t="inlineStr">
+        <is>
+          <t>E/One</t>
+        </is>
+      </c>
+      <c r="C21" t="inlineStr">
+        <is>
+          <t>Grinder Pumps</t>
+        </is>
+      </c>
+      <c r="D21" t="inlineStr">
+        <is>
           <t>Flow Control</t>
         </is>
       </c>
@@ -583,33 +898,86 @@
     <row r="22">
       <c r="A22" t="inlineStr">
         <is>
-          <t>Flow Control</t>
+          <t>Example Rep Firm</t>
+        </is>
+      </c>
+      <c r="B22" t="inlineStr">
+        <is>
+          <t>Lakeside Equipment</t>
+        </is>
+      </c>
+      <c r="C22" t="inlineStr">
+        <is>
+          <t>Equipment for all stages of wastewater treatment</t>
+        </is>
+      </c>
+      <c r="D22" t="inlineStr">
+        <is>
+          <t>Wastewater Treatment</t>
         </is>
       </c>
     </row>
     <row r="23">
       <c r="A23" t="inlineStr">
         <is>
-          <t>Wastewater Treatment</t>
+          <t>Example Rep Firm</t>
+        </is>
+      </c>
+      <c r="B23" t="inlineStr">
+        <is>
+          <t>Next Turbo</t>
+        </is>
+      </c>
+      <c r="C23" t="inlineStr">
+        <is>
+          <t>Geared Turbo Compressors</t>
+        </is>
+      </c>
+      <c r="D23" t="inlineStr">
+        <is>
+          <t>Aeration</t>
         </is>
       </c>
     </row>
     <row r="24">
       <c r="A24" t="inlineStr">
         <is>
-          <t>Aeration</t>
+          <t>Example Rep Firm</t>
+        </is>
+      </c>
+      <c r="B24" t="inlineStr">
+        <is>
+          <t>USF Fabrication</t>
+        </is>
+      </c>
+      <c r="C24" t="inlineStr">
+        <is>
+          <t>Aluminum Access Hatches</t>
+        </is>
+      </c>
+      <c r="D24" t="inlineStr">
+        <is>
+          <t>Water Treatment</t>
         </is>
       </c>
     </row>
     <row r="25">
       <c r="A25" t="inlineStr">
         <is>
-          <t>Water Treatment</t>
-        </is>
-      </c>
-    </row>
-    <row r="26">
-      <c r="A26" t="inlineStr">
+          <t>Example Rep Firm</t>
+        </is>
+      </c>
+      <c r="B25" t="inlineStr">
+        <is>
+          <t>USF Fabrication</t>
+        </is>
+      </c>
+      <c r="C25" t="inlineStr">
+        <is>
+          <t>Fall Through Safety Grate System</t>
+        </is>
+      </c>
+      <c r="D25" t="inlineStr">
         <is>
           <t>Water Treatment</t>
         </is>

</xml_diff>

<commit_message>
added comma handling to ChatGPT prompt
</commit_message>
<xml_diff>
--- a/example_output.xlsx
+++ b/example_output.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:D25"/>
+  <dimension ref="A1:D39"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -458,528 +458,836 @@
     <row r="2">
       <c r="A2" t="inlineStr">
         <is>
-          <t>Example Rep Firm</t>
+          <t>Treatment Technologies</t>
         </is>
       </c>
       <c r="B2" t="inlineStr">
         <is>
-          <t>ABB</t>
+          <t>JWC Environmental</t>
         </is>
       </c>
       <c r="C2" t="inlineStr">
         <is>
-          <t>Variable Frequency Drives</t>
+          <t>Muffin Monster</t>
         </is>
       </c>
       <c r="D2" t="inlineStr">
         <is>
-          <t>Flow Control</t>
+          <t>Screening</t>
         </is>
       </c>
     </row>
     <row r="3">
       <c r="A3" t="inlineStr">
         <is>
-          <t>Example Rep Firm</t>
+          <t>Treatment Technologies</t>
         </is>
       </c>
       <c r="B3" t="inlineStr">
         <is>
-          <t>Old Castle</t>
+          <t>JWC Environmental</t>
         </is>
       </c>
       <c r="C3" t="inlineStr">
         <is>
-          <t>One Lift Package Pump Station</t>
+          <t>Channel Monster</t>
         </is>
       </c>
       <c r="D3" t="inlineStr">
         <is>
-          <t>Flow Control</t>
+          <t>Screening</t>
         </is>
       </c>
     </row>
     <row r="4">
       <c r="A4" t="inlineStr">
         <is>
-          <t>Example Rep Firm</t>
+          <t>Treatment Technologies</t>
         </is>
       </c>
       <c r="B4" t="inlineStr">
         <is>
-          <t>Netzsch</t>
+          <t>JWC Environmental</t>
         </is>
       </c>
       <c r="C4" t="inlineStr">
         <is>
-          <t>Progressive Cavity Pumps</t>
+          <t>Auger Monster</t>
         </is>
       </c>
       <c r="D4" t="inlineStr">
         <is>
-          <t>Flow Control</t>
+          <t>Screening</t>
         </is>
       </c>
     </row>
     <row r="5">
       <c r="A5" t="inlineStr">
         <is>
-          <t>Example Rep Firm</t>
+          <t>Treatment Technologies</t>
         </is>
       </c>
       <c r="B5" t="inlineStr">
         <is>
-          <t>Netzsch</t>
+          <t>JWC Environmental</t>
         </is>
       </c>
       <c r="C5" t="inlineStr">
         <is>
-          <t>Rotary Lobe Pumps</t>
+          <t>Fine Screens</t>
         </is>
       </c>
       <c r="D5" t="inlineStr">
         <is>
-          <t>Flow Control</t>
+          <t>Screening</t>
         </is>
       </c>
     </row>
     <row r="6">
       <c r="A6" t="inlineStr">
         <is>
-          <t>Example Rep Firm</t>
+          <t>Treatment Technologies</t>
         </is>
       </c>
       <c r="B6" t="inlineStr">
         <is>
-          <t>USCP</t>
+          <t>JWC Environmental</t>
         </is>
       </c>
       <c r="C6" t="inlineStr">
         <is>
-          <t>Steel Reinforced Polymer Concrete Manholes</t>
+          <t>Band Screens</t>
         </is>
       </c>
       <c r="D6" t="inlineStr">
         <is>
-          <t>Water Treatment</t>
+          <t>Screening</t>
         </is>
       </c>
     </row>
     <row r="7">
       <c r="A7" t="inlineStr">
         <is>
-          <t>Example Rep Firm</t>
+          <t>Treatment Technologies</t>
         </is>
       </c>
       <c r="B7" t="inlineStr">
         <is>
-          <t>USCP</t>
+          <t>JWC Environmental</t>
         </is>
       </c>
       <c r="C7" t="inlineStr">
         <is>
-          <t>Microtunnel Pipe</t>
+          <t>Drum Screens</t>
         </is>
       </c>
       <c r="D7" t="inlineStr">
         <is>
-          <t>Water Treatment</t>
+          <t>Screening</t>
         </is>
       </c>
     </row>
     <row r="8">
       <c r="A8" t="inlineStr">
         <is>
-          <t>Example Rep Firm</t>
+          <t>Treatment Technologies</t>
         </is>
       </c>
       <c r="B8" t="inlineStr">
         <is>
-          <t>USCP</t>
+          <t>JWC Environmental</t>
         </is>
       </c>
       <c r="C8" t="inlineStr">
         <is>
-          <t>Industrial Pipe Structures</t>
+          <t>Strom Screens</t>
         </is>
       </c>
       <c r="D8" t="inlineStr">
         <is>
-          <t>Water Treatment</t>
+          <t>Screening</t>
         </is>
       </c>
     </row>
     <row r="9">
       <c r="A9" t="inlineStr">
         <is>
-          <t>Example Rep Firm</t>
+          <t>Treatment Technologies</t>
         </is>
       </c>
       <c r="B9" t="inlineStr">
         <is>
-          <t>Flygt</t>
+          <t>JWC Environmental</t>
         </is>
       </c>
       <c r="C9" t="inlineStr">
         <is>
-          <t>Submersible Pumps</t>
+          <t>Screening Washer Monster</t>
         </is>
       </c>
       <c r="D9" t="inlineStr">
         <is>
-          <t>Flow Control</t>
+          <t>Screening</t>
         </is>
       </c>
     </row>
     <row r="10">
       <c r="A10" t="inlineStr">
         <is>
-          <t>Example Rep Firm</t>
+          <t>Treatment Technologies</t>
         </is>
       </c>
       <c r="B10" t="inlineStr">
         <is>
-          <t>Flygt</t>
+          <t>JWC Environmental</t>
         </is>
       </c>
       <c r="C10" t="inlineStr">
         <is>
-          <t>Submersible Mixers</t>
+          <t>Honey Monster Septage Receiving Station</t>
         </is>
       </c>
       <c r="D10" t="inlineStr">
         <is>
-          <t>Aeration</t>
+          <t>Grease and FOG Removal</t>
         </is>
       </c>
     </row>
     <row r="11">
       <c r="A11" t="inlineStr">
         <is>
-          <t>Example Rep Firm</t>
+          <t>Treatment Technologies</t>
         </is>
       </c>
       <c r="B11" t="inlineStr">
         <is>
-          <t>Flygt</t>
+          <t>IPEC</t>
         </is>
       </c>
       <c r="C11" t="inlineStr">
         <is>
-          <t>Controls</t>
+          <t>Rotary Drum Sludge Thickeners</t>
         </is>
       </c>
       <c r="D11" t="inlineStr">
         <is>
-          <t>Flow Control</t>
+          <t>Clarification</t>
         </is>
       </c>
     </row>
     <row r="12">
       <c r="A12" t="inlineStr">
         <is>
-          <t>Example Rep Firm</t>
+          <t>Treatment Technologies</t>
         </is>
       </c>
       <c r="B12" t="inlineStr">
         <is>
-          <t>Flygt</t>
+          <t>IPEC</t>
         </is>
       </c>
       <c r="C12" t="inlineStr">
         <is>
-          <t>Check Valves</t>
+          <t>Internally-Fed Rotary Screens</t>
         </is>
       </c>
       <c r="D12" t="inlineStr">
         <is>
-          <t>Flow Control</t>
+          <t>Screening</t>
         </is>
       </c>
     </row>
     <row r="13">
       <c r="A13" t="inlineStr">
         <is>
-          <t>Example Rep Firm</t>
+          <t>Treatment Technologies</t>
         </is>
       </c>
       <c r="B13" t="inlineStr">
         <is>
-          <t>Flygt</t>
+          <t>IPEC</t>
         </is>
       </c>
       <c r="C13" t="inlineStr">
         <is>
-          <t>Mix-Flush Valves</t>
+          <t>Static Screens</t>
         </is>
       </c>
       <c r="D13" t="inlineStr">
         <is>
-          <t>Flow Control</t>
+          <t>Screening</t>
         </is>
       </c>
     </row>
     <row r="14">
       <c r="A14" t="inlineStr">
         <is>
-          <t>Example Rep Firm</t>
+          <t>Treatment Technologies</t>
         </is>
       </c>
       <c r="B14" t="inlineStr">
         <is>
-          <t>ITT Gould Pumps</t>
+          <t>FRC Systems International</t>
         </is>
       </c>
       <c r="C14" t="inlineStr">
         <is>
-          <t>Standard Cast Iron Pumps</t>
+          <t>Dissolved Air Floatation (DAF)</t>
         </is>
       </c>
       <c r="D14" t="inlineStr">
         <is>
-          <t>Flow Control</t>
+          <t>Clarification</t>
         </is>
       </c>
     </row>
     <row r="15">
       <c r="A15" t="inlineStr">
         <is>
-          <t>Example Rep Firm</t>
+          <t>Treatment Technologies</t>
         </is>
       </c>
       <c r="B15" t="inlineStr">
         <is>
-          <t>ITT Gould Pumps</t>
+          <t>V-Fold</t>
         </is>
       </c>
       <c r="C15" t="inlineStr">
         <is>
-          <t>Bronze Pumps</t>
+          <t>Sludge Dewatering</t>
         </is>
       </c>
       <c r="D15" t="inlineStr">
         <is>
-          <t>Flow Control</t>
+          <t>Filtration</t>
         </is>
       </c>
     </row>
     <row r="16">
       <c r="A16" t="inlineStr">
         <is>
-          <t>Example Rep Firm</t>
+          <t>Treatment Technologies</t>
         </is>
       </c>
       <c r="B16" t="inlineStr">
         <is>
-          <t>ITT Gould Pumps</t>
+          <t>Chemco Systems</t>
         </is>
       </c>
       <c r="C16" t="inlineStr">
         <is>
-          <t>End Suction Pumps</t>
+          <t>Powder Activated Carbon</t>
         </is>
       </c>
       <c r="D16" t="inlineStr">
         <is>
-          <t>Flow Control</t>
+          <t>Chemical Feed</t>
         </is>
       </c>
     </row>
     <row r="17">
       <c r="A17" t="inlineStr">
         <is>
-          <t>Example Rep Firm</t>
+          <t>Treatment Technologies</t>
         </is>
       </c>
       <c r="B17" t="inlineStr">
         <is>
-          <t>ITT Gould Pumps</t>
+          <t>Chemco Systems</t>
         </is>
       </c>
       <c r="C17" t="inlineStr">
         <is>
-          <t>Vertical Turbine Pumps</t>
+          <t>Lime Slacker</t>
         </is>
       </c>
       <c r="D17" t="inlineStr">
         <is>
-          <t>Flow Control</t>
+          <t>Chemical Feed</t>
         </is>
       </c>
     </row>
     <row r="18">
       <c r="A18" t="inlineStr">
         <is>
-          <t>Example Rep Firm</t>
+          <t>Treatment Technologies</t>
         </is>
       </c>
       <c r="B18" t="inlineStr">
         <is>
-          <t>ITT Gould Pumps</t>
+          <t>Chemco Systems</t>
         </is>
       </c>
       <c r="C18" t="inlineStr">
         <is>
-          <t>Split Case Pumps</t>
+          <t>Hydrated Lime</t>
         </is>
       </c>
       <c r="D18" t="inlineStr">
         <is>
-          <t>Flow Control</t>
+          <t>Chemical Feed</t>
         </is>
       </c>
     </row>
     <row r="19">
       <c r="A19" t="inlineStr">
         <is>
-          <t>Example Rep Firm</t>
+          <t>Treatment Technologies</t>
         </is>
       </c>
       <c r="B19" t="inlineStr">
         <is>
-          <t>E/One</t>
+          <t>Chemco Systems</t>
         </is>
       </c>
       <c r="C19" t="inlineStr">
         <is>
-          <t>Packaged Low Pressure Sewer Systems</t>
+          <t>Soda Ash</t>
         </is>
       </c>
       <c r="D19" t="inlineStr">
         <is>
-          <t>Flow Control</t>
+          <t>Chemical Feed</t>
         </is>
       </c>
     </row>
     <row r="20">
       <c r="A20" t="inlineStr">
         <is>
-          <t>Example Rep Firm</t>
+          <t>Treatment Technologies</t>
         </is>
       </c>
       <c r="B20" t="inlineStr">
         <is>
-          <t>E/One</t>
+          <t>Chemco Systems</t>
         </is>
       </c>
       <c r="C20" t="inlineStr">
         <is>
-          <t>Collection Basin</t>
+          <t>Bulk Bag Unloader</t>
         </is>
       </c>
       <c r="D20" t="inlineStr">
         <is>
-          <t>Flow Control</t>
+          <t>Chemical Feed</t>
         </is>
       </c>
     </row>
     <row r="21">
       <c r="A21" t="inlineStr">
         <is>
-          <t>Example Rep Firm</t>
+          <t>Treatment Technologies</t>
         </is>
       </c>
       <c r="B21" t="inlineStr">
         <is>
-          <t>E/One</t>
+          <t>Chemco Systems</t>
         </is>
       </c>
       <c r="C21" t="inlineStr">
         <is>
-          <t>Grinder Pumps</t>
+          <t>Silo Systems</t>
         </is>
       </c>
       <c r="D21" t="inlineStr">
         <is>
-          <t>Flow Control</t>
+          <t>Chemical Feed</t>
         </is>
       </c>
     </row>
     <row r="22">
       <c r="A22" t="inlineStr">
         <is>
-          <t>Example Rep Firm</t>
+          <t>Treatment Technologies</t>
         </is>
       </c>
       <c r="B22" t="inlineStr">
         <is>
-          <t>Lakeside Equipment</t>
+          <t>Clearas</t>
         </is>
       </c>
       <c r="C22" t="inlineStr">
         <is>
-          <t>Equipment for all stages of wastewater treatment</t>
+          <t>Advanced Biological Nutrient Recovery (ABNR) technology</t>
         </is>
       </c>
       <c r="D22" t="inlineStr">
         <is>
-          <t>Wastewater Treatment</t>
+          <t>Nutrient Recovery</t>
         </is>
       </c>
     </row>
     <row r="23">
       <c r="A23" t="inlineStr">
         <is>
-          <t>Example Rep Firm</t>
+          <t>Treatment Technologies</t>
         </is>
       </c>
       <c r="B23" t="inlineStr">
         <is>
-          <t>Next Turbo</t>
+          <t>Fibracast</t>
         </is>
       </c>
       <c r="C23" t="inlineStr">
         <is>
-          <t>Geared Turbo Compressors</t>
+          <t>FibrePlate Membrane Bioreactor (MBR) Technology</t>
         </is>
       </c>
       <c r="D23" t="inlineStr">
         <is>
-          <t>Aeration</t>
+          <t>Filtration</t>
         </is>
       </c>
     </row>
     <row r="24">
       <c r="A24" t="inlineStr">
         <is>
-          <t>Example Rep Firm</t>
+          <t>Treatment Technologies</t>
         </is>
       </c>
       <c r="B24" t="inlineStr">
         <is>
-          <t>USF Fabrication</t>
+          <t>Kruger</t>
         </is>
       </c>
       <c r="C24" t="inlineStr">
         <is>
-          <t>Aluminum Access Hatches</t>
+          <t>Phased Oxidation Ditches</t>
         </is>
       </c>
       <c r="D24" t="inlineStr">
         <is>
-          <t>Water Treatment</t>
+          <t>Aeration</t>
         </is>
       </c>
     </row>
     <row r="25">
       <c r="A25" t="inlineStr">
         <is>
-          <t>Example Rep Firm</t>
+          <t>Treatment Technologies</t>
         </is>
       </c>
       <c r="B25" t="inlineStr">
         <is>
-          <t>USF Fabrication</t>
+          <t>Kruger</t>
         </is>
       </c>
       <c r="C25" t="inlineStr">
         <is>
-          <t>Fall Through Safety Grate System</t>
+          <t>Discfilter</t>
         </is>
       </c>
       <c r="D25" t="inlineStr">
         <is>
-          <t>Water Treatment</t>
+          <t>Filtration</t>
+        </is>
+      </c>
+    </row>
+    <row r="26">
+      <c r="A26" t="inlineStr">
+        <is>
+          <t>Treatment Technologies</t>
+        </is>
+      </c>
+      <c r="B26" t="inlineStr">
+        <is>
+          <t>Kruger</t>
+        </is>
+      </c>
+      <c r="C26" t="inlineStr">
+        <is>
+          <t>BioCon Thermal Dryer</t>
+        </is>
+      </c>
+      <c r="D26" t="inlineStr">
+        <is>
+          <t>Sludge Management</t>
+        </is>
+      </c>
+    </row>
+    <row r="27">
+      <c r="A27" t="inlineStr">
+        <is>
+          <t>Treatment Technologies</t>
+        </is>
+      </c>
+      <c r="B27" t="inlineStr">
+        <is>
+          <t>Kruger</t>
+        </is>
+      </c>
+      <c r="C27" t="inlineStr">
+        <is>
+          <t>ACTIFLO</t>
+        </is>
+      </c>
+      <c r="D27" t="inlineStr">
+        <is>
+          <t>Clarification</t>
+        </is>
+      </c>
+    </row>
+    <row r="28">
+      <c r="A28" t="inlineStr">
+        <is>
+          <t>Treatment Technologies</t>
+        </is>
+      </c>
+      <c r="B28" t="inlineStr">
+        <is>
+          <t>DTE Environmental</t>
+        </is>
+      </c>
+      <c r="C28" t="inlineStr">
+        <is>
+          <t>Grit Classifier</t>
+        </is>
+      </c>
+      <c r="D28" t="inlineStr">
+        <is>
+          <t>Screening</t>
+        </is>
+      </c>
+    </row>
+    <row r="29">
+      <c r="A29" t="inlineStr">
+        <is>
+          <t>Treatment Technologies</t>
+        </is>
+      </c>
+      <c r="B29" t="inlineStr">
+        <is>
+          <t>Rodney Hunt</t>
+        </is>
+      </c>
+      <c r="C29" t="inlineStr">
+        <is>
+          <t>Sluice Gates</t>
+        </is>
+      </c>
+      <c r="D29" t="inlineStr">
+        <is>
+          <t>Flow Control</t>
+        </is>
+      </c>
+    </row>
+    <row r="30">
+      <c r="A30" t="inlineStr">
+        <is>
+          <t>Treatment Technologies</t>
+        </is>
+      </c>
+      <c r="B30" t="inlineStr">
+        <is>
+          <t>Rodney Hunt</t>
+        </is>
+      </c>
+      <c r="C30" t="inlineStr">
+        <is>
+          <t>Slide Gates</t>
+        </is>
+      </c>
+      <c r="D30" t="inlineStr">
+        <is>
+          <t>Flow Control</t>
+        </is>
+      </c>
+    </row>
+    <row r="31">
+      <c r="A31" t="inlineStr">
+        <is>
+          <t>Treatment Technologies</t>
+        </is>
+      </c>
+      <c r="B31" t="inlineStr">
+        <is>
+          <t>Entek Technologies</t>
+        </is>
+      </c>
+      <c r="C31" t="inlineStr">
+        <is>
+          <t>Aeration Systems</t>
+        </is>
+      </c>
+      <c r="D31" t="inlineStr">
+        <is>
+          <t>Aeration</t>
+        </is>
+      </c>
+    </row>
+    <row r="32">
+      <c r="A32" t="inlineStr">
+        <is>
+          <t>Treatment Technologies</t>
+        </is>
+      </c>
+      <c r="B32" t="inlineStr">
+        <is>
+          <t>BNR Systems</t>
+        </is>
+      </c>
+      <c r="C32" t="inlineStr">
+        <is>
+          <t>Shaftless Spiral Conveyors</t>
+        </is>
+      </c>
+      <c r="D32" t="inlineStr">
+        <is>
+          <t>Sludge Management</t>
+        </is>
+      </c>
+    </row>
+    <row r="33">
+      <c r="A33" t="inlineStr">
+        <is>
+          <t>Treatment Technologies</t>
+        </is>
+      </c>
+      <c r="B33" t="inlineStr">
+        <is>
+          <t>BNR Systems</t>
+        </is>
+      </c>
+      <c r="C33" t="inlineStr">
+        <is>
+          <t>Live Bottom Hoppers</t>
+        </is>
+      </c>
+      <c r="D33" t="inlineStr">
+        <is>
+          <t>Sludge Management</t>
+        </is>
+      </c>
+    </row>
+    <row r="34">
+      <c r="A34" t="inlineStr">
+        <is>
+          <t>Treatment Technologies</t>
+        </is>
+      </c>
+      <c r="B34" t="inlineStr">
+        <is>
+          <t>BNR Systems</t>
+        </is>
+      </c>
+      <c r="C34" t="inlineStr">
+        <is>
+          <t>Chain and Rake Screens</t>
+        </is>
+      </c>
+      <c r="D34" t="inlineStr">
+        <is>
+          <t>Screening</t>
+        </is>
+      </c>
+    </row>
+    <row r="35">
+      <c r="A35" t="inlineStr">
+        <is>
+          <t>Treatment Technologies</t>
+        </is>
+      </c>
+      <c r="B35" t="inlineStr">
+        <is>
+          <t>BNR Systems</t>
+        </is>
+      </c>
+      <c r="C35" t="inlineStr">
+        <is>
+          <t>Fine Screens</t>
+        </is>
+      </c>
+      <c r="D35" t="inlineStr">
+        <is>
+          <t>Screening</t>
+        </is>
+      </c>
+    </row>
+    <row r="36">
+      <c r="A36" t="inlineStr">
+        <is>
+          <t>Treatment Technologies</t>
+        </is>
+      </c>
+      <c r="B36" t="inlineStr">
+        <is>
+          <t>BNR Systems</t>
+        </is>
+      </c>
+      <c r="C36" t="inlineStr">
+        <is>
+          <t>Packages Headwork Systems for Screening and Grit Removal</t>
+        </is>
+      </c>
+      <c r="D36" t="inlineStr">
+        <is>
+          <t>Screening</t>
+        </is>
+      </c>
+    </row>
+    <row r="37">
+      <c r="A37" t="inlineStr">
+        <is>
+          <t>Treatment Technologies</t>
+        </is>
+      </c>
+      <c r="B37" t="inlineStr">
+        <is>
+          <t>BNR Systems</t>
+        </is>
+      </c>
+      <c r="C37" t="inlineStr">
+        <is>
+          <t>Grit Vortek</t>
+        </is>
+      </c>
+      <c r="D37" t="inlineStr">
+        <is>
+          <t>Screening</t>
+        </is>
+      </c>
+    </row>
+    <row r="38">
+      <c r="A38" t="inlineStr">
+        <is>
+          <t>Treatment Technologies</t>
+        </is>
+      </c>
+      <c r="B38" t="inlineStr">
+        <is>
+          <t>BNR Systems</t>
+        </is>
+      </c>
+      <c r="C38" t="inlineStr">
+        <is>
+          <t>Grit Classifier</t>
+        </is>
+      </c>
+      <c r="D38" t="inlineStr">
+        <is>
+          <t>Screening</t>
+        </is>
+      </c>
+    </row>
+    <row r="39">
+      <c r="A39" t="inlineStr">
+        <is>
+          <t>Treatment Technologies</t>
+        </is>
+      </c>
+      <c r="B39" t="inlineStr">
+        <is>
+          <t>BNR Systems</t>
+        </is>
+      </c>
+      <c r="C39" t="inlineStr">
+        <is>
+          <t>Screenings Washer</t>
+        </is>
+      </c>
+      <c r="D39" t="inlineStr">
+        <is>
+          <t>Screening</t>
         </is>
       </c>
     </row>

</xml_diff>